<commit_message>
adjustet comments for 1 ghost tag
</commit_message>
<xml_diff>
--- a/WGFP_GhostTags.xlsx
+++ b/WGFP_GhostTags.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3934" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3934" uniqueCount="183">
   <si>
     <t>TagID</t>
   </si>
@@ -576,6 +576,9 @@
   </si>
   <si>
     <t>Likely ghost, Mature fish at tagging; likely spawned out tag in October 2021, though hard to tell if before or after 10-19-21 detections (not really a spwning location); best guess is that detection on 4-19-22 is spawning location in good gravel riffle (and ghost date), with downstream movement between 2022 and 2023 caused by high floods in spring 2023</t>
+  </si>
+  <si>
+    <t>Likely Ghost; Big fish when tagged; upstream movement after release likely back to capture location and probably spawned in that same location shortly after being tagged (ghost tag date of 7-28-21); ghost tag downstream movement due to high flows between 4-20-22 and 7-26-23</t>
   </si>
 </sst>
 </file>
@@ -1519,7 +1522,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A249" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I252" sqref="I252"/>
+      <selection pane="bottomLeft" activeCell="Q261" sqref="Q261"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17838,8 +17841,8 @@
       <c r="S263" s="1">
         <v>0</v>
       </c>
-      <c r="T263" s="1" t="s">
-        <v>19</v>
+      <c r="T263" s="2" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="264" spans="1:20" x14ac:dyDescent="0.3">
@@ -18526,6 +18529,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -18533,8 +18537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N388"/>
   <sheetViews>
-    <sheetView topLeftCell="A357" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD388"/>
+    <sheetView topLeftCell="A279" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K295" sqref="K295"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18544,6 +18548,7 @@
     <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -18662,10 +18667,10 @@
       <c r="K7" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="M7" t="s">
+      <c r="M7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N7" t="s">
+      <c r="N7" s="2" t="s">
         <v>30</v>
       </c>
     </row>
@@ -18703,10 +18708,10 @@
       <c r="K8" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="M8">
+      <c r="M8" s="2">
         <v>7</v>
       </c>
-      <c r="N8">
+      <c r="N8" s="2">
         <f>COUNTIF($I$8:$I$388, M8)</f>
         <v>13</v>
       </c>
@@ -18745,10 +18750,10 @@
       <c r="K9" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="M9">
+      <c r="M9" s="2">
         <v>6</v>
       </c>
-      <c r="N9" s="1">
+      <c r="N9" s="2">
         <f>COUNTIF($I$8:$I$388, M9)</f>
         <v>20</v>
       </c>
@@ -18787,10 +18792,10 @@
       <c r="K10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="M10">
+      <c r="M10" s="2">
         <v>5</v>
       </c>
-      <c r="N10" s="1">
+      <c r="N10" s="2">
         <f>COUNTIF($I$8:$I$388, M10)</f>
         <v>59</v>
       </c>
@@ -18829,10 +18834,10 @@
       <c r="K11" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="M11">
+      <c r="M11" s="2">
         <v>4</v>
       </c>
-      <c r="N11" s="1">
+      <c r="N11" s="2">
         <f>COUNTIF($I$8:$I$388, M11)</f>
         <v>106</v>
       </c>
@@ -18871,10 +18876,10 @@
       <c r="K12" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="M12">
+      <c r="M12" s="2">
         <v>3</v>
       </c>
-      <c r="N12" s="1">
+      <c r="N12" s="2">
         <f>COUNTIF($I$8:$I$388, M12)</f>
         <v>183</v>
       </c>
@@ -18913,7 +18918,6 @@
       <c r="K13" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="N13" s="1"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
@@ -18949,7 +18953,6 @@
       <c r="K14" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="N14" s="1"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
@@ -18985,7 +18988,6 @@
       <c r="K15" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="N15" s="1"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
@@ -25217,7 +25219,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="194" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A194" s="5">
         <v>230000272636</v>
       </c>
@@ -28752,39 +28754,39 @@
         <v>141</v>
       </c>
     </row>
-    <row r="295" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A295" s="17">
+    <row r="295" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A295" s="10">
         <v>230000272949</v>
       </c>
-      <c r="B295" s="2">
-        <v>0</v>
-      </c>
-      <c r="C295" s="2">
-        <v>0</v>
-      </c>
-      <c r="D295" s="2">
-        <v>1</v>
-      </c>
-      <c r="E295" s="2">
-        <v>1</v>
-      </c>
-      <c r="F295" s="2">
-        <v>1</v>
-      </c>
-      <c r="G295" s="2">
-        <v>0</v>
-      </c>
-      <c r="H295" s="2">
-        <v>1</v>
-      </c>
-      <c r="I295" s="2">
+      <c r="B295" s="11">
+        <v>0</v>
+      </c>
+      <c r="C295" s="11">
+        <v>0</v>
+      </c>
+      <c r="D295" s="11">
+        <v>1</v>
+      </c>
+      <c r="E295" s="11">
+        <v>1</v>
+      </c>
+      <c r="F295" s="11">
+        <v>1</v>
+      </c>
+      <c r="G295" s="11">
+        <v>0</v>
+      </c>
+      <c r="H295" s="11">
+        <v>1</v>
+      </c>
+      <c r="I295" s="11">
         <v>4</v>
       </c>
-      <c r="J295" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="K295" s="2" t="s">
-        <v>174</v>
+      <c r="J295" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="K295" s="11" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="296" spans="1:11" x14ac:dyDescent="0.3">
@@ -30362,7 +30364,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="341" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A341" s="5">
         <v>226001581552</v>
       </c>
@@ -30397,7 +30399,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="342" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A342" s="5">
         <v>230000228037</v>
       </c>
@@ -30432,7 +30434,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="343" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A343" s="10">
         <v>230000224169</v>
       </c>
@@ -30467,7 +30469,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="344" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A344" s="5">
         <v>230000228087</v>
       </c>
@@ -30502,7 +30504,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="345" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A345" s="5">
         <v>230000272076</v>
       </c>
@@ -30537,7 +30539,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="346" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A346" s="5">
         <v>230000272735</v>
       </c>
@@ -30572,7 +30574,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="347" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A347" s="5">
         <v>230000228979</v>
       </c>
@@ -30607,7 +30609,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="348" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A348" s="5">
         <v>230000228414</v>
       </c>
@@ -30642,7 +30644,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="349" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A349" s="5">
         <v>230000228613</v>
       </c>
@@ -30677,7 +30679,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="350" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A350" s="5">
         <v>230000228991</v>
       </c>
@@ -30712,7 +30714,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="351" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A351" s="5">
         <v>230000142993</v>
       </c>
@@ -30747,7 +30749,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="352" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A352" s="5">
         <v>230000224158</v>
       </c>
@@ -30782,7 +30784,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="353" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A353" s="5">
         <v>230000224556</v>
       </c>
@@ -30817,7 +30819,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="354" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A354" s="5">
         <v>230000272038</v>
       </c>
@@ -30852,7 +30854,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="355" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A355" s="5">
         <v>230000228356</v>
       </c>
@@ -30887,7 +30889,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="356" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A356" s="5">
         <v>230000224449</v>
       </c>
@@ -30922,7 +30924,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="357" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A357" s="5">
         <v>226001581628</v>
       </c>
@@ -30957,7 +30959,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="358" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A358" s="5">
         <v>230000228352</v>
       </c>
@@ -30992,7 +30994,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="359" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A359" s="5">
         <v>230000272867</v>
       </c>
@@ -31027,7 +31029,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="360" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A360" s="5">
         <v>230000229036</v>
       </c>
@@ -31062,7 +31064,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="361" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A361" s="12">
         <v>226001581554</v>
       </c>
@@ -31097,7 +31099,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="362" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A362" s="12">
         <v>230000224357</v>
       </c>
@@ -31132,7 +31134,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="363" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A363" s="10">
         <v>230000224360</v>
       </c>
@@ -31167,7 +31169,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="364" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A364" s="5">
         <v>230000224387</v>
       </c>
@@ -31202,7 +31204,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="365" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A365" s="12">
         <v>230000224473</v>
       </c>
@@ -31237,7 +31239,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="366" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A366" s="12">
         <v>230000228063</v>
       </c>
@@ -31272,7 +31274,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="367" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A367" s="12">
         <v>230000228065</v>
       </c>
@@ -31307,7 +31309,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="368" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A368" s="12">
         <v>230000228580</v>
       </c>
@@ -31342,7 +31344,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="369" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A369" s="12">
         <v>230000228679</v>
       </c>
@@ -31377,7 +31379,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="370" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A370" s="12">
         <v>230000228728</v>
       </c>
@@ -31412,7 +31414,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="371" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A371" s="12">
         <v>230000228830</v>
       </c>
@@ -31447,7 +31449,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="372" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A372" s="12">
         <v>230000228930</v>
       </c>
@@ -31482,7 +31484,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="373" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A373" s="12">
         <v>230000229042</v>
       </c>
@@ -31517,7 +31519,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="374" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A374" s="10">
         <v>230000272004</v>
       </c>
@@ -31552,7 +31554,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="375" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A375" s="5">
         <v>230000272033</v>
       </c>
@@ -31587,7 +31589,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="376" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A376" s="12">
         <v>230000272064</v>
       </c>
@@ -31622,7 +31624,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="377" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A377" s="17">
         <v>230000272099</v>
       </c>
@@ -31657,7 +31659,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="378" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A378" s="12">
         <v>230000272230</v>
       </c>
@@ -31692,7 +31694,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="379" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A379" s="12">
         <v>230000272240</v>
       </c>
@@ -31727,7 +31729,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="380" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A380" s="12">
         <v>230000272260</v>
       </c>
@@ -31762,7 +31764,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="381" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A381" s="12">
         <v>230000272360</v>
       </c>
@@ -31797,7 +31799,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="382" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A382" s="12">
         <v>230000272364</v>
       </c>
@@ -31832,7 +31834,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="383" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A383" s="17">
         <v>230000272557</v>
       </c>
@@ -31867,7 +31869,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="384" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A384" s="12">
         <v>230000272685</v>
       </c>
@@ -31902,7 +31904,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="385" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A385" s="12">
         <v>230000272699</v>
       </c>
@@ -31937,7 +31939,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="386" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A386" s="12">
         <v>230000272870</v>
       </c>
@@ -31972,7 +31974,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="387" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A387" s="5">
         <v>230000272966</v>
       </c>
@@ -32007,7 +32009,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="388" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A388" s="12">
         <v>230000272989</v>
       </c>

</xml_diff>